<commit_message>
BurdonChart 2.3v y 3v
</commit_message>
<xml_diff>
--- a/Proyecto/Documentacion/PREGAME/1. ELICITACION/1.6 Backlog/G4_Backlog-Sprint_v2.1.xlsx
+++ b/Proyecto/Documentacion/PREGAME/1. ELICITACION/1.6 Backlog/G4_Backlog-Sprint_v2.1.xlsx
@@ -1,34 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\7185_G4\Proyecto\Documentacion\PREGAME\1. ELICITACION\1.6 Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panch\Desktop\University\Semester-VI\Analisis\7185_G4\Proyecto\Documentacion\PREGAME\1. ELICITACION\1.6 Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6AAD6D-016B-41FF-B74D-730888CC4DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE663FAA-2BA3-4EDD-B231-D692F7B45CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog" sheetId="2" r:id="rId2"/>
     <sheet name="sprint1" sheetId="3" r:id="rId3"/>
     <sheet name="sprint2" sheetId="5" r:id="rId4"/>
-    <sheet name="burdonchart-spring1" sheetId="4" r:id="rId5"/>
-    <sheet name="burdonchart-spring2" sheetId="6" r:id="rId6"/>
+    <sheet name="burdonchart-sprint1" sheetId="4" r:id="rId5"/>
+    <sheet name="burdonchart-sprint2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$H$13</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="150">
   <si>
     <t>Prioridad</t>
   </si>
@@ -483,12 +485,18 @@
   <si>
     <t>Habilitar la base de datos para la eliminacion del cliente</t>
   </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>Las horas trabajadas, fueron menor que la planificacion, pudiendo observar, que el modulo, fue concluido antes de lo planificado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -536,6 +544,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -593,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -631,15 +646,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -648,8 +667,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,6 +749,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'burdonchart-sprint1'!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -737,31 +770,36 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Hora Estimada Restantet</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burdonchart-spring1'!$B$24:$H$24</c:f>
+              <c:f>'burdonchart-sprint1'!$C$24:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -777,6 +815,18 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'burdonchart-sprint1'!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Estimadas
+Restantes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -787,31 +837,36 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Hora Estimada Restantet</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burdonchart-spring1'!$B$25:$H$25</c:f>
+              <c:f>'burdonchart-sprint1'!$C$25:$H$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1017,6 +1072,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'burdonchart-sprint2'!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Estimadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1029,7 +1095,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burdonchart-spring2'!$D$20:$I$20</c:f>
+              <c:f>'burdonchart-sprint2'!$D$20:$I$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1056,7 +1122,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burdonchart-spring2'!$D$19:$I$19</c:f>
+              <c:f>'burdonchart-sprint2'!$D$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1091,6 +1157,18 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'burdonchart-sprint2'!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Horas Estimadas
+Restantes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1103,7 +1181,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burdonchart-spring2'!$D$20:$I$20</c:f>
+              <c:f>'burdonchart-sprint2'!$D$20:$I$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1130,7 +1208,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burdonchart-spring2'!$D$20:$I$20</c:f>
+              <c:f>'burdonchart-sprint2'!$D$20:$I$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1694,13 +1772,15 @@
   </sheetPr>
   <dimension ref="A1:H793"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="A11:H11"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="62.140625" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
@@ -1736,7 +1816,7 @@
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -3091,8 +3171,8 @@
   </sheetPr>
   <dimension ref="A1:Z931"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:F49"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I49" sqref="I47:I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3296,12 +3376,12 @@
         <f>CONCATENATE(B4,"_",A6)</f>
         <v>REQ001_1</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="4" t="s">
         <v>7</v>
       </c>
@@ -3335,12 +3415,12 @@
         <f>CONCATENATE(B4,"_",A7)</f>
         <v>REQ001_2</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="4" t="s">
         <v>7</v>
       </c>
@@ -3374,12 +3454,12 @@
         <f>CONCATENATE(B4,"_",A8)</f>
         <v>REQ001_3</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="4" t="s">
         <v>7</v>
       </c>
@@ -3408,10 +3488,10 @@
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -3436,10 +3516,10 @@
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -3599,12 +3679,12 @@
         <f>CONCATENATE(B12,"_",A14)</f>
         <v>REQ002_1</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="4" t="s">
         <v>7</v>
       </c>
@@ -3638,12 +3718,12 @@
         <f>CONCATENATE(B12,"_",A15)</f>
         <v>REQ002_2</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="4" t="s">
         <v>7</v>
       </c>
@@ -3677,12 +3757,12 @@
         <f>CONCATENATE(B12,"_",A16)</f>
         <v>REQ002_3</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="4" t="s">
         <v>7</v>
       </c>
@@ -3902,12 +3982,12 @@
         <f>CONCATENATE(B20,"_",A22)</f>
         <v>REQ003_1</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="4" t="s">
         <v>7</v>
       </c>
@@ -3941,12 +4021,12 @@
         <f>CONCATENATE(B20,"_",A23)</f>
         <v>REQ003_2</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="4" t="s">
         <v>7</v>
       </c>
@@ -3980,12 +4060,12 @@
         <f>CONCATENATE(B20,"_",A24)</f>
         <v>REQ003_3</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="4" t="s">
         <v>7</v>
       </c>
@@ -4205,12 +4285,12 @@
         <f>CONCATENATE(B28,"_",A30)</f>
         <v>REQ004_1</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="4" t="s">
         <v>7</v>
       </c>
@@ -4244,12 +4324,12 @@
         <f>CONCATENATE(B28,"_",A31)</f>
         <v>REQ004_2</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="4" t="s">
         <v>7</v>
       </c>
@@ -4283,12 +4363,12 @@
         <f>CONCATENATE(B28,"_",A32)</f>
         <v>REQ004_3</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="4" t="s">
         <v>7</v>
       </c>
@@ -4508,12 +4588,12 @@
         <f>CONCATENATE(B36,"_",A38)</f>
         <v>REQ005_1</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
       <c r="G38" s="4" t="s">
         <v>7</v>
       </c>
@@ -4547,12 +4627,12 @@
         <f>CONCATENATE(B36,"_",A39)</f>
         <v>REQ005_2</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
       <c r="G39" s="4" t="s">
         <v>7</v>
       </c>
@@ -4586,12 +4666,12 @@
         <f>CONCATENATE(B36,"_",A40)</f>
         <v>REQ005_3</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
       <c r="G40" s="4" t="s">
         <v>7</v>
       </c>
@@ -4625,12 +4705,12 @@
         <f>CONCATENATE(B36,"_",A41)</f>
         <v>REQ005_4</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
       <c r="G41" s="4" t="s">
         <v>7</v>
       </c>
@@ -4850,12 +4930,12 @@
         <f>CONCATENATE(B45,"_",A47)</f>
         <v>REQ006_1</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
       <c r="G47" s="4" t="s">
         <v>7</v>
       </c>
@@ -4889,12 +4969,12 @@
         <f>CONCATENATE(B45,"_",A48)</f>
         <v>REQ006_2</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
       <c r="G48" s="4" t="s">
         <v>7</v>
       </c>
@@ -4928,12 +5008,12 @@
         <f>CONCATENATE(B45,"_",A49)</f>
         <v>REQ006_3</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
       <c r="G49" s="4" t="s">
         <v>7</v>
       </c>
@@ -29700,8 +29780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AF3BD5-229C-40B4-B2E3-EFEE31A879A4}">
   <dimension ref="A3:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29777,12 +29857,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="8" t="s">
         <v>109</v>
       </c>
@@ -29799,12 +29879,12 @@
         <f>CONCATENATE(B4,"_",A6)</f>
         <v>REQ007_1</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
@@ -29821,12 +29901,12 @@
         <f>CONCATENATE(B4,"_",A7)</f>
         <v>REQ007_2</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
@@ -29843,12 +29923,12 @@
         <f>CONCATENATE(B4,"_",A8)</f>
         <v>REQ007_3</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="4" t="s">
         <v>10</v>
       </c>
@@ -29858,10 +29938,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="8"/>
       <c r="H9" s="5"/>
       <c r="I9" s="8"/>
@@ -29927,12 +30007,12 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
       <c r="G14" s="8" t="s">
         <v>109</v>
       </c>
@@ -29949,12 +30029,12 @@
         <f>CONCATENATE(B13,"_",A15)</f>
         <v>REQ008_1</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="4" t="s">
         <v>10</v>
       </c>
@@ -29971,12 +30051,12 @@
         <f>CONCATENATE(B13,"_",A16)</f>
         <v>REQ008_2</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="4" t="s">
         <v>10</v>
       </c>
@@ -29993,12 +30073,12 @@
         <f>CONCATENATE(B13,"_",A17)</f>
         <v>REQ008_3</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="4" t="s">
         <v>10</v>
       </c>
@@ -30015,12 +30095,12 @@
         <f>CONCATENATE(B13,"_",A18)</f>
         <v>REQ008_4</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="4" t="s">
         <v>10</v>
       </c>
@@ -30090,12 +30170,12 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
       <c r="G23" s="8" t="s">
         <v>109</v>
       </c>
@@ -30112,12 +30192,12 @@
         <f>CONCATENATE(B22,"_",A24)</f>
         <v>REQ009_1</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="4" t="s">
         <v>10</v>
       </c>
@@ -30134,12 +30214,12 @@
         <f>CONCATENATE(B22,"_",A25)</f>
         <v>REQ009_2</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="4" t="s">
         <v>10</v>
       </c>
@@ -30156,12 +30236,12 @@
         <f>CONCATENATE(B22,"_",A26)</f>
         <v>REQ009_3</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="4" t="s">
         <v>10</v>
       </c>
@@ -30178,12 +30258,12 @@
         <f>CONCATENATE(B22,"_",A27)</f>
         <v>REQ009_4</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="4" t="s">
         <v>10</v>
       </c>
@@ -30200,12 +30280,12 @@
         <f>CONCATENATE(B22,"_",A28)</f>
         <v>REQ009_5</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="4" t="s">
         <v>10</v>
       </c>
@@ -30275,12 +30355,12 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
       <c r="G33" s="8" t="s">
         <v>109</v>
       </c>
@@ -30297,12 +30377,12 @@
         <f>CONCATENATE(B32,"_",A34)</f>
         <v>REQ010_1</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="4" t="s">
         <v>10</v>
       </c>
@@ -30319,12 +30399,12 @@
         <f>CONCATENATE(B32,"_",A35)</f>
         <v>REQ010_2</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="4" t="s">
         <v>10</v>
       </c>
@@ -30341,12 +30421,12 @@
         <f>CONCATENATE(B32,"_",A36)</f>
         <v>REQ010_3</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="4" t="s">
         <v>10</v>
       </c>
@@ -30355,10 +30435,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -30408,8 +30488,8 @@
   </sheetPr>
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31488,7 +31568,7 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="33" t="s">
         <v>135</v>
       </c>
       <c r="C25" s="16">
@@ -31546,14 +31626,16 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
+      <c r="L26" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
@@ -31574,14 +31656,16 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
+      <c r="L27" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
@@ -58583,6 +58667,10 @@
       <c r="Z991" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L26:S26"/>
+    <mergeCell ref="L27:S27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -58594,10 +58682,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AD0B63-AC3F-471E-B34D-1DFEBD2B4B52}">
-  <dimension ref="C3:J20"/>
+  <dimension ref="C3:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -58607,6 +58695,7 @@
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="7.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="22" max="22" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.2">
@@ -59010,7 +59099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C17" s="11" t="str">
         <f>sprint2!B36</f>
         <v>REQ010_3</v>
@@ -59039,7 +59128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C19" s="14" t="s">
         <v>134</v>
       </c>
@@ -59068,7 +59157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C20" s="14" t="s">
         <v>135</v>
       </c>
@@ -59097,11 +59186,40 @@
         <v>11.2</v>
       </c>
     </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="O25" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="O26" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="O25:V25"/>
+    <mergeCell ref="O26:V26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>